<commit_message>
Made compatible with updates to breakpoint definition code.
</commit_message>
<xml_diff>
--- a/dataIn/dataSourceList.xlsx
+++ b/dataIn/dataSourceList.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Agency</t>
   </si>
@@ -55,9 +54,6 @@
     <t>ME</t>
   </si>
   <si>
-    <t>MTUSGS</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -68,14 +64,52 @@
   </si>
   <si>
     <t>West</t>
+  </si>
+  <si>
+    <t>MTUSGSGlacier</t>
+  </si>
+  <si>
+    <t>MTUSGSYellowstone</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Robert Al-Chokhachy</t>
+  </si>
+  <si>
+    <t>MEFRO</t>
+  </si>
+  <si>
+    <t>Jed Wright</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Waiting for Daymet update to pair air temp</t>
+  </si>
+  <si>
+    <t>Ben Letcher</t>
+  </si>
+  <si>
+    <t>Leslie Jones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -99,12 +133,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,107 +457,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated plots & code
</commit_message>
<xml_diff>
--- a/dataIn/dataSourceList.xlsx
+++ b/dataIn/dataSourceList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Agency</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>Leslie Jones</t>
+  </si>
+  <si>
+    <t>USFS</t>
+  </si>
+  <si>
+    <t>MA + VT</t>
+  </si>
+  <si>
+    <t>Keith Nislow</t>
+  </si>
+  <si>
+    <t>MAOARS</t>
+  </si>
+  <si>
+    <t>Matt O'Donnell</t>
+  </si>
+  <si>
+    <t>Raw data, need to process (~ 5-10 sites)</t>
+  </si>
+  <si>
+    <t>No location data</t>
   </si>
 </sst>
 </file>
@@ -457,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,22 +537,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -544,35 +563,37 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -583,28 +604,28 @@
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -613,9 +634,45 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed problematic commits. Attempt to update all folders.
</commit_message>
<xml_diff>
--- a/dataIn/dataSourceList.xlsx
+++ b/dataIn/dataSourceList.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Source List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Agency</t>
   </si>
@@ -115,6 +113,27 @@
   </si>
   <si>
     <t>No location data</t>
+  </si>
+  <si>
+    <t>VTFWS</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Austin Polebitski</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Untouched</t>
+  </si>
+  <si>
+    <t>Preparation Status</t>
   </si>
 </sst>
 </file>
@@ -138,15 +157,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,20 +206,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -478,21 +538,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,198 +570,209 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="H2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>